<commit_message>
updating to XLS 0.6.16, XLSX 0.5.15
</commit_message>
<xml_diff>
--- a/test_files/openpyxl_r_formulae.xlsx
+++ b/test_files/openpyxl_r_formulae.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6500" yWindow="1560" windowWidth="24480" windowHeight="17260" tabRatio="500"/>
@@ -97,9 +97,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -428,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
@@ -562,6 +562,12 @@
       </c>
       <c r="C14">
         <v>605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="str">
+        <f>IF(ISBLANK(B16), "Düsseldorf", B16)</f>
+        <v>Düsseldorf</v>
       </c>
     </row>
   </sheetData>

</xml_diff>